<commit_message>
02.06 add sequence diagram
</commit_message>
<xml_diff>
--- a/docs/assets/Tables.xlsx
+++ b/docs/assets/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Обучение\mkdocs\project\docs\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD51F7E-8BE6-4E77-8857-DB2FA988ECA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC6714F-B117-4151-ACC4-3E7628E9BBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DD698DF6-4024-46AF-A1D9-13F852030986}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="14" xr2:uid="{DD698DF6-4024-46AF-A1D9-13F852030986}"/>
   </bookViews>
   <sheets>
     <sheet name="Глоссарий" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="130">
   <si>
     <t>ЛК</t>
   </si>
@@ -838,6 +838,9 @@
   </si>
   <si>
     <t>![](../diagrams/out/auth.svg){ width="100" }</t>
+  </si>
+  <si>
+    <t>![](../diagrams/out/booking_table.svg){ width="100" }</t>
   </si>
 </sst>
 </file>
@@ -1774,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159E9D95-E196-43CA-936B-39EC843CC12D}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,6 +1843,14 @@
       </c>
       <c r="B7" s="3" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +2003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7AC94C-EE25-49E7-AF69-50456E05F153}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2145,7 +2156,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
03.06 update sequense diagrams
</commit_message>
<xml_diff>
--- a/docs/assets/Tables.xlsx
+++ b/docs/assets/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Обучение\mkdocs\project\docs\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC6714F-B117-4151-ACC4-3E7628E9BBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFC7107-2802-49E2-AB94-4F3529CDDF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="14" xr2:uid="{DD698DF6-4024-46AF-A1D9-13F852030986}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="132">
   <si>
     <t>ЛК</t>
   </si>
@@ -841,6 +841,12 @@
   </si>
   <si>
     <t>![](../diagrams/out/booking_table.svg){ width="100" }</t>
+  </si>
+  <si>
+    <t>![](../diagrams/out/registration_client.svg){ width="100" }</t>
+  </si>
+  <si>
+    <t>![](../diagrams/out/registration_user.svg){ width="100" }</t>
   </si>
 </sst>
 </file>
@@ -1544,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CC5513-12F9-4A3B-82E7-7A4D610CEEE8}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,6 +1616,14 @@
       </c>
       <c r="B7" s="5" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1780,7 +1794,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7AC94C-EE25-49E7-AF69-50456E05F153}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,6 +2082,14 @@
       </c>
       <c r="B7" s="5" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>